<commit_message>
Include a "modules" column.
</commit_message>
<xml_diff>
--- a/data/ecological_attributes.xlsx
+++ b/data/ecological_attributes.xlsx
@@ -12,7 +12,7 @@
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$AD$191</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$AE$191</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
@@ -505,12 +505,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="AE1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Florencia Miguel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+name of modules where trees are when doing modularity index</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="235">
   <si>
     <t>trees</t>
   </si>
@@ -1191,6 +1215,30 @@
   </si>
   <si>
     <t>H.shannon</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>F</t>
+  </si>
+  <si>
+    <t>modules</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -1568,11 +1616,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD191"/>
+  <dimension ref="A1:AE191"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J12" sqref="J12"/>
+      <selection pane="bottomLeft" activeCell="AF6" sqref="AF6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1597,8 +1645,8 @@
     <col min="18" max="18" width="7.28515625" customWidth="1"/>
     <col min="19" max="19" width="6.5703125" customWidth="1"/>
     <col min="20" max="21" width="7" customWidth="1"/>
-    <col min="22" max="22" width="8.7109375" style="3" customWidth="1"/>
-    <col min="23" max="23" width="9.42578125" style="3" customWidth="1"/>
+    <col min="22" max="22" width="7.28515625" style="3" customWidth="1"/>
+    <col min="23" max="23" width="8" style="3" customWidth="1"/>
     <col min="24" max="24" width="4.85546875" customWidth="1"/>
     <col min="25" max="25" width="5.28515625" customWidth="1"/>
     <col min="26" max="26" width="4.7109375" customWidth="1"/>
@@ -1606,9 +1654,10 @@
     <col min="28" max="28" width="4.5703125" customWidth="1"/>
     <col min="29" max="29" width="7.5703125" customWidth="1"/>
     <col min="30" max="30" width="9.42578125" customWidth="1"/>
+    <col min="31" max="31" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30">
+    <row r="1" spans="1:31">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1699,8 +1748,11 @@
       <c r="AD1" t="s">
         <v>225</v>
       </c>
+      <c r="AE1" t="s">
+        <v>233</v>
+      </c>
     </row>
-    <row r="2" spans="1:30">
+    <row r="2" spans="1:31">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1791,8 +1843,11 @@
       <c r="AD2" s="7">
         <v>6232314</v>
       </c>
+      <c r="AE2" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="3" spans="1:30">
+    <row r="3" spans="1:31">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1883,8 +1938,11 @@
       <c r="AD3" s="7">
         <v>6232314</v>
       </c>
+      <c r="AE3" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="4" spans="1:30">
+    <row r="4" spans="1:31">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1975,8 +2033,11 @@
       <c r="AD4" s="7">
         <v>6232314</v>
       </c>
+      <c r="AE4" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="5" spans="1:30">
+    <row r="5" spans="1:31">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -2067,8 +2128,11 @@
       <c r="AD5" s="7">
         <v>6232314</v>
       </c>
+      <c r="AE5" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="6" spans="1:30">
+    <row r="6" spans="1:31">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -2159,8 +2223,11 @@
       <c r="AD6" s="7">
         <v>6232314</v>
       </c>
+      <c r="AE6" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="7" spans="1:30">
+    <row r="7" spans="1:31">
       <c r="A7" t="s">
         <v>11</v>
       </c>
@@ -2251,8 +2318,11 @@
       <c r="AD7" s="7">
         <v>6232314</v>
       </c>
+      <c r="AE7" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="8" spans="1:30">
+    <row r="8" spans="1:31">
       <c r="A8" t="s">
         <v>12</v>
       </c>
@@ -2343,8 +2413,11 @@
       <c r="AD8" s="7">
         <v>6232314</v>
       </c>
+      <c r="AE8" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="9" spans="1:30">
+    <row r="9" spans="1:31">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -2435,8 +2508,11 @@
       <c r="AD9" s="7">
         <v>6232314</v>
       </c>
+      <c r="AE9" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="10" spans="1:30">
+    <row r="10" spans="1:31">
       <c r="A10" t="s">
         <v>14</v>
       </c>
@@ -2527,8 +2603,11 @@
       <c r="AD10" s="7">
         <v>6231077</v>
       </c>
+      <c r="AE10" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="11" spans="1:30">
+    <row r="11" spans="1:31">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -2619,8 +2698,11 @@
       <c r="AD11" s="7">
         <v>6231077</v>
       </c>
+      <c r="AE11" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="12" spans="1:30">
+    <row r="12" spans="1:31">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -2711,8 +2793,11 @@
       <c r="AD12" s="7">
         <v>6231077</v>
       </c>
+      <c r="AE12" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="13" spans="1:30">
+    <row r="13" spans="1:31">
       <c r="A13" t="s">
         <v>17</v>
       </c>
@@ -2803,8 +2888,11 @@
       <c r="AD13" s="7">
         <v>6231077</v>
       </c>
+      <c r="AE13" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="14" spans="1:30">
+    <row r="14" spans="1:31">
       <c r="A14" t="s">
         <v>18</v>
       </c>
@@ -2895,8 +2983,11 @@
       <c r="AD14" s="7">
         <v>6231077</v>
       </c>
+      <c r="AE14" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="15" spans="1:30">
+    <row r="15" spans="1:31">
       <c r="A15" t="s">
         <v>19</v>
       </c>
@@ -2987,8 +3078,11 @@
       <c r="AD15" s="7">
         <v>6231077</v>
       </c>
+      <c r="AE15" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="16" spans="1:30">
+    <row r="16" spans="1:31">
       <c r="A16" t="s">
         <v>20</v>
       </c>
@@ -3079,8 +3173,11 @@
       <c r="AD16" s="7">
         <v>6231077</v>
       </c>
+      <c r="AE16" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="17" spans="1:30">
+    <row r="17" spans="1:31">
       <c r="A17" t="s">
         <v>21</v>
       </c>
@@ -3171,8 +3268,11 @@
       <c r="AD17" s="7">
         <v>6231077</v>
       </c>
+      <c r="AE17" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="18" spans="1:30">
+    <row r="18" spans="1:31">
       <c r="A18" t="s">
         <v>22</v>
       </c>
@@ -3263,8 +3363,11 @@
       <c r="AD18" s="7">
         <v>6229175</v>
       </c>
+      <c r="AE18" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="19" spans="1:30">
+    <row r="19" spans="1:31">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -3355,8 +3458,11 @@
       <c r="AD19" s="7">
         <v>6229175</v>
       </c>
+      <c r="AE19" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="20" spans="1:30">
+    <row r="20" spans="1:31">
       <c r="A20" t="s">
         <v>24</v>
       </c>
@@ -3447,8 +3553,11 @@
       <c r="AD20" s="7">
         <v>6229175</v>
       </c>
+      <c r="AE20" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="21" spans="1:30">
+    <row r="21" spans="1:31">
       <c r="A21" t="s">
         <v>25</v>
       </c>
@@ -3539,8 +3648,11 @@
       <c r="AD21" s="7">
         <v>6229175</v>
       </c>
+      <c r="AE21" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="22" spans="1:30">
+    <row r="22" spans="1:31">
       <c r="A22" t="s">
         <v>26</v>
       </c>
@@ -3631,8 +3743,11 @@
       <c r="AD22" s="7">
         <v>6229175</v>
       </c>
+      <c r="AE22" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="23" spans="1:30">
+    <row r="23" spans="1:31">
       <c r="A23" t="s">
         <v>27</v>
       </c>
@@ -3723,8 +3838,11 @@
       <c r="AD23" s="7">
         <v>6230727</v>
       </c>
+      <c r="AE23" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="24" spans="1:30">
+    <row r="24" spans="1:31">
       <c r="A24" t="s">
         <v>28</v>
       </c>
@@ -3815,8 +3933,11 @@
       <c r="AD24" s="7">
         <v>6230727</v>
       </c>
+      <c r="AE24" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="25" spans="1:30">
+    <row r="25" spans="1:31">
       <c r="A25" t="s">
         <v>29</v>
       </c>
@@ -3907,8 +4028,11 @@
       <c r="AD25" s="7">
         <v>6230727</v>
       </c>
+      <c r="AE25" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="26" spans="1:30">
+    <row r="26" spans="1:31">
       <c r="A26" t="s">
         <v>30</v>
       </c>
@@ -3999,8 +4123,11 @@
       <c r="AD26" s="7">
         <v>6228247</v>
       </c>
+      <c r="AE26" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="27" spans="1:30">
+    <row r="27" spans="1:31">
       <c r="A27" t="s">
         <v>31</v>
       </c>
@@ -4091,8 +4218,11 @@
       <c r="AD27" s="7">
         <v>6228247</v>
       </c>
+      <c r="AE27" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="28" spans="1:30">
+    <row r="28" spans="1:31">
       <c r="A28" t="s">
         <v>32</v>
       </c>
@@ -4183,8 +4313,11 @@
       <c r="AD28" s="7">
         <v>6228247</v>
       </c>
+      <c r="AE28" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="29" spans="1:30">
+    <row r="29" spans="1:31">
       <c r="A29" t="s">
         <v>33</v>
       </c>
@@ -4275,8 +4408,11 @@
       <c r="AD29" s="7">
         <v>6228247</v>
       </c>
+      <c r="AE29" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="30" spans="1:30">
+    <row r="30" spans="1:31">
       <c r="A30" t="s">
         <v>34</v>
       </c>
@@ -4367,8 +4503,11 @@
       <c r="AD30" s="7">
         <v>6228229</v>
       </c>
+      <c r="AE30" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="31" spans="1:30">
+    <row r="31" spans="1:31">
       <c r="A31" t="s">
         <v>35</v>
       </c>
@@ -4459,8 +4598,11 @@
       <c r="AD31" s="7">
         <v>6228229</v>
       </c>
+      <c r="AE31" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="32" spans="1:30">
+    <row r="32" spans="1:31">
       <c r="A32" t="s">
         <v>36</v>
       </c>
@@ -4551,8 +4693,11 @@
       <c r="AD32" s="7">
         <v>6228229</v>
       </c>
+      <c r="AE32" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="33" spans="1:30">
+    <row r="33" spans="1:31">
       <c r="A33" t="s">
         <v>37</v>
       </c>
@@ -4643,8 +4788,11 @@
       <c r="AD33" s="7">
         <v>6228229</v>
       </c>
+      <c r="AE33" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="34" spans="1:30">
+    <row r="34" spans="1:31">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -4735,8 +4883,11 @@
       <c r="AD34" s="7">
         <v>6229959</v>
       </c>
+      <c r="AE34" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="35" spans="1:30">
+    <row r="35" spans="1:31">
       <c r="A35" t="s">
         <v>39</v>
       </c>
@@ -4827,8 +4978,11 @@
       <c r="AD35" s="7">
         <v>6229959</v>
       </c>
+      <c r="AE35" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="36" spans="1:30">
+    <row r="36" spans="1:31">
       <c r="A36" t="s">
         <v>40</v>
       </c>
@@ -4919,8 +5073,11 @@
       <c r="AD36" s="7">
         <v>6229959</v>
       </c>
+      <c r="AE36" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="37" spans="1:30">
+    <row r="37" spans="1:31">
       <c r="A37" t="s">
         <v>41</v>
       </c>
@@ -5011,8 +5168,11 @@
       <c r="AD37" s="7">
         <v>6229959</v>
       </c>
+      <c r="AE37" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="38" spans="1:30">
+    <row r="38" spans="1:31">
       <c r="A38" t="s">
         <v>42</v>
       </c>
@@ -5103,8 +5263,11 @@
       <c r="AD38" s="7">
         <v>6229959</v>
       </c>
+      <c r="AE38" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="39" spans="1:30">
+    <row r="39" spans="1:31">
       <c r="A39" t="s">
         <v>43</v>
       </c>
@@ -5195,8 +5358,11 @@
       <c r="AD39" s="7">
         <v>6229959</v>
       </c>
+      <c r="AE39" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="40" spans="1:30">
+    <row r="40" spans="1:31">
       <c r="A40" t="s">
         <v>44</v>
       </c>
@@ -5287,8 +5453,11 @@
       <c r="AD40" s="7">
         <v>6229959</v>
       </c>
+      <c r="AE40" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="41" spans="1:30">
+    <row r="41" spans="1:31">
       <c r="A41" t="s">
         <v>45</v>
       </c>
@@ -5379,8 +5548,11 @@
       <c r="AD41" s="7">
         <v>6229959</v>
       </c>
+      <c r="AE41" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="42" spans="1:30">
+    <row r="42" spans="1:31">
       <c r="A42" t="s">
         <v>46</v>
       </c>
@@ -5471,8 +5643,11 @@
       <c r="AD42" s="7">
         <v>6230231</v>
       </c>
+      <c r="AE42" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="43" spans="1:30">
+    <row r="43" spans="1:31">
       <c r="A43" t="s">
         <v>47</v>
       </c>
@@ -5563,8 +5738,11 @@
       <c r="AD43" s="7">
         <v>6230231</v>
       </c>
+      <c r="AE43" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="44" spans="1:30">
+    <row r="44" spans="1:31">
       <c r="A44" t="s">
         <v>48</v>
       </c>
@@ -5655,8 +5833,11 @@
       <c r="AD44" s="7">
         <v>6230231</v>
       </c>
+      <c r="AE44" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="45" spans="1:30">
+    <row r="45" spans="1:31">
       <c r="A45" t="s">
         <v>49</v>
       </c>
@@ -5747,8 +5928,11 @@
       <c r="AD45" s="7">
         <v>6230231</v>
       </c>
+      <c r="AE45" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="46" spans="1:30">
+    <row r="46" spans="1:31">
       <c r="A46" t="s">
         <v>50</v>
       </c>
@@ -5839,8 +6023,11 @@
       <c r="AD46" s="7">
         <v>6230231</v>
       </c>
+      <c r="AE46" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="47" spans="1:30">
+    <row r="47" spans="1:31">
       <c r="A47" t="s">
         <v>51</v>
       </c>
@@ -5931,8 +6118,11 @@
       <c r="AD47" s="7">
         <v>6230231</v>
       </c>
+      <c r="AE47" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="48" spans="1:30">
+    <row r="48" spans="1:31">
       <c r="A48" t="s">
         <v>52</v>
       </c>
@@ -6023,8 +6213,11 @@
       <c r="AD48" s="7">
         <v>6230231</v>
       </c>
+      <c r="AE48" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="49" spans="1:30">
+    <row r="49" spans="1:31">
       <c r="A49" t="s">
         <v>53</v>
       </c>
@@ -6115,8 +6308,11 @@
       <c r="AD49" s="7">
         <v>6230231</v>
       </c>
+      <c r="AE49" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="50" spans="1:30">
+    <row r="50" spans="1:31">
       <c r="A50" t="s">
         <v>54</v>
       </c>
@@ -6207,8 +6403,11 @@
       <c r="AD50" s="7">
         <v>6229745</v>
       </c>
+      <c r="AE50" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="51" spans="1:30">
+    <row r="51" spans="1:31">
       <c r="A51" t="s">
         <v>55</v>
       </c>
@@ -6299,8 +6498,11 @@
       <c r="AD51" s="7">
         <v>6229745</v>
       </c>
+      <c r="AE51" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="52" spans="1:30">
+    <row r="52" spans="1:31">
       <c r="A52" t="s">
         <v>56</v>
       </c>
@@ -6391,8 +6593,11 @@
       <c r="AD52" s="7">
         <v>6229745</v>
       </c>
+      <c r="AE52" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="53" spans="1:30">
+    <row r="53" spans="1:31">
       <c r="A53" t="s">
         <v>57</v>
       </c>
@@ -6483,8 +6688,11 @@
       <c r="AD53" s="7">
         <v>6229745</v>
       </c>
+      <c r="AE53" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="54" spans="1:30">
+    <row r="54" spans="1:31">
       <c r="A54" t="s">
         <v>58</v>
       </c>
@@ -6575,8 +6783,11 @@
       <c r="AD54" s="7">
         <v>6229745</v>
       </c>
+      <c r="AE54" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="55" spans="1:30">
+    <row r="55" spans="1:31">
       <c r="A55" t="s">
         <v>59</v>
       </c>
@@ -6667,8 +6878,11 @@
       <c r="AD55" s="7">
         <v>6229745</v>
       </c>
+      <c r="AE55" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="56" spans="1:30">
+    <row r="56" spans="1:31">
       <c r="A56" t="s">
         <v>60</v>
       </c>
@@ -6759,8 +6973,11 @@
       <c r="AD56" s="7">
         <v>6231024</v>
       </c>
+      <c r="AE56" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="57" spans="1:30">
+    <row r="57" spans="1:31">
       <c r="A57" t="s">
         <v>61</v>
       </c>
@@ -6851,8 +7068,11 @@
       <c r="AD57" s="7">
         <v>6231024</v>
       </c>
+      <c r="AE57" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="58" spans="1:30">
+    <row r="58" spans="1:31">
       <c r="A58" t="s">
         <v>62</v>
       </c>
@@ -6943,8 +7163,11 @@
       <c r="AD58" s="7">
         <v>6231024</v>
       </c>
+      <c r="AE58" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="59" spans="1:30">
+    <row r="59" spans="1:31">
       <c r="A59" t="s">
         <v>63</v>
       </c>
@@ -7035,8 +7258,11 @@
       <c r="AD59" s="7">
         <v>6231024</v>
       </c>
+      <c r="AE59" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="60" spans="1:30">
+    <row r="60" spans="1:31">
       <c r="A60" t="s">
         <v>64</v>
       </c>
@@ -7127,8 +7353,11 @@
       <c r="AD60" s="7">
         <v>6231024</v>
       </c>
+      <c r="AE60" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="61" spans="1:30">
+    <row r="61" spans="1:31">
       <c r="A61" t="s">
         <v>65</v>
       </c>
@@ -7219,8 +7448,11 @@
       <c r="AD61" s="7">
         <v>6231024</v>
       </c>
+      <c r="AE61" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="62" spans="1:30">
+    <row r="62" spans="1:31">
       <c r="A62" t="s">
         <v>66</v>
       </c>
@@ -7311,8 +7543,11 @@
       <c r="AD62" s="7">
         <v>6234208</v>
       </c>
+      <c r="AE62" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="63" spans="1:30">
+    <row r="63" spans="1:31">
       <c r="A63" t="s">
         <v>68</v>
       </c>
@@ -7403,8 +7638,11 @@
       <c r="AD63" s="7">
         <v>6234208</v>
       </c>
+      <c r="AE63" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="64" spans="1:30">
+    <row r="64" spans="1:31">
       <c r="A64" t="s">
         <v>69</v>
       </c>
@@ -7495,8 +7733,11 @@
       <c r="AD64" s="7">
         <v>6234208</v>
       </c>
+      <c r="AE64" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="65" spans="1:30">
+    <row r="65" spans="1:31">
       <c r="A65" t="s">
         <v>70</v>
       </c>
@@ -7587,8 +7828,11 @@
       <c r="AD65" s="7">
         <v>6234208</v>
       </c>
+      <c r="AE65" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="66" spans="1:30">
+    <row r="66" spans="1:31">
       <c r="A66" t="s">
         <v>71</v>
       </c>
@@ -7679,8 +7923,11 @@
       <c r="AD66" s="7">
         <v>6234208</v>
       </c>
+      <c r="AE66" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="67" spans="1:30">
+    <row r="67" spans="1:31">
       <c r="A67" t="s">
         <v>72</v>
       </c>
@@ -7771,8 +8018,11 @@
       <c r="AD67" s="7">
         <v>6234208</v>
       </c>
+      <c r="AE67" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="68" spans="1:30">
+    <row r="68" spans="1:31">
       <c r="A68" t="s">
         <v>73</v>
       </c>
@@ -7863,8 +8113,11 @@
       <c r="AD68" s="7">
         <v>6234208</v>
       </c>
+      <c r="AE68" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="69" spans="1:30">
+    <row r="69" spans="1:31">
       <c r="A69" t="s">
         <v>74</v>
       </c>
@@ -7955,8 +8208,11 @@
       <c r="AD69" s="7">
         <v>6234257</v>
       </c>
+      <c r="AE69" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="70" spans="1:30">
+    <row r="70" spans="1:31">
       <c r="A70" t="s">
         <v>75</v>
       </c>
@@ -8047,8 +8303,11 @@
       <c r="AD70" s="7">
         <v>6234257</v>
       </c>
+      <c r="AE70" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="71" spans="1:30">
+    <row r="71" spans="1:31">
       <c r="A71" t="s">
         <v>76</v>
       </c>
@@ -8139,8 +8398,11 @@
       <c r="AD71" s="7">
         <v>6234257</v>
       </c>
+      <c r="AE71" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="72" spans="1:30">
+    <row r="72" spans="1:31">
       <c r="A72" t="s">
         <v>77</v>
       </c>
@@ -8231,8 +8493,11 @@
       <c r="AD72" s="7">
         <v>6234281</v>
       </c>
+      <c r="AE72" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="73" spans="1:30">
+    <row r="73" spans="1:31">
       <c r="A73" t="s">
         <v>78</v>
       </c>
@@ -8323,8 +8588,11 @@
       <c r="AD73" s="7">
         <v>6234276</v>
       </c>
+      <c r="AE73" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="74" spans="1:30">
+    <row r="74" spans="1:31">
       <c r="A74" t="s">
         <v>79</v>
       </c>
@@ -8415,8 +8683,11 @@
       <c r="AD74" s="7">
         <v>6234276</v>
       </c>
+      <c r="AE74" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="75" spans="1:30">
+    <row r="75" spans="1:31">
       <c r="A75" t="s">
         <v>80</v>
       </c>
@@ -8507,8 +8778,11 @@
       <c r="AD75" s="7">
         <v>6234276</v>
       </c>
+      <c r="AE75" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="76" spans="1:30">
+    <row r="76" spans="1:31">
       <c r="A76" t="s">
         <v>81</v>
       </c>
@@ -8599,8 +8873,11 @@
       <c r="AD76" s="7">
         <v>6234276</v>
       </c>
+      <c r="AE76" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="77" spans="1:30">
+    <row r="77" spans="1:31">
       <c r="A77" t="s">
         <v>82</v>
       </c>
@@ -8691,8 +8968,11 @@
       <c r="AD77" s="7">
         <v>6232277</v>
       </c>
+      <c r="AE77" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="78" spans="1:30">
+    <row r="78" spans="1:31">
       <c r="A78" t="s">
         <v>83</v>
       </c>
@@ -8783,8 +9063,11 @@
       <c r="AD78" s="7">
         <v>6232264</v>
       </c>
+      <c r="AE78" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="79" spans="1:30">
+    <row r="79" spans="1:31">
       <c r="A79" t="s">
         <v>84</v>
       </c>
@@ -8875,8 +9158,11 @@
       <c r="AD79" s="7">
         <v>6232235</v>
       </c>
+      <c r="AE79" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="80" spans="1:30">
+    <row r="80" spans="1:31">
       <c r="A80" t="s">
         <v>85</v>
       </c>
@@ -8967,8 +9253,11 @@
       <c r="AD80" s="7">
         <v>6232235</v>
       </c>
+      <c r="AE80" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="81" spans="1:30">
+    <row r="81" spans="1:31">
       <c r="A81" t="s">
         <v>86</v>
       </c>
@@ -9059,8 +9348,11 @@
       <c r="AD81" s="7">
         <v>6232235</v>
       </c>
+      <c r="AE81" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="82" spans="1:30">
+    <row r="82" spans="1:31">
       <c r="A82" t="s">
         <v>87</v>
       </c>
@@ -9151,8 +9443,11 @@
       <c r="AD82" s="8">
         <v>6232254</v>
       </c>
+      <c r="AE82" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="83" spans="1:30">
+    <row r="83" spans="1:31">
       <c r="A83" t="s">
         <v>88</v>
       </c>
@@ -9243,8 +9538,11 @@
       <c r="AD83" s="8">
         <v>6232254</v>
       </c>
+      <c r="AE83" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="84" spans="1:30">
+    <row r="84" spans="1:31">
       <c r="A84" t="s">
         <v>89</v>
       </c>
@@ -9335,8 +9633,11 @@
       <c r="AD84" s="8">
         <v>6232254</v>
       </c>
+      <c r="AE84" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="85" spans="1:30">
+    <row r="85" spans="1:31">
       <c r="A85" t="s">
         <v>90</v>
       </c>
@@ -9427,8 +9728,11 @@
       <c r="AD85" s="8">
         <v>6232254</v>
       </c>
+      <c r="AE85" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="86" spans="1:30">
+    <row r="86" spans="1:31">
       <c r="A86" t="s">
         <v>91</v>
       </c>
@@ -9519,8 +9823,11 @@
       <c r="AD86" s="8">
         <v>6232254</v>
       </c>
+      <c r="AE86" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="87" spans="1:30">
+    <row r="87" spans="1:31">
       <c r="A87" t="s">
         <v>92</v>
       </c>
@@ -9611,8 +9918,11 @@
       <c r="AD87" s="8">
         <v>6232254</v>
       </c>
+      <c r="AE87" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="88" spans="1:30">
+    <row r="88" spans="1:31">
       <c r="A88" t="s">
         <v>93</v>
       </c>
@@ -9703,8 +10013,11 @@
       <c r="AD88" s="8">
         <v>6232254</v>
       </c>
+      <c r="AE88" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="89" spans="1:30">
+    <row r="89" spans="1:31">
       <c r="A89" t="s">
         <v>94</v>
       </c>
@@ -9795,8 +10108,11 @@
       <c r="AD89" s="8">
         <v>6232254</v>
       </c>
+      <c r="AE89" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="90" spans="1:30">
+    <row r="90" spans="1:31">
       <c r="A90" t="s">
         <v>95</v>
       </c>
@@ -9887,8 +10203,11 @@
       <c r="AD90" s="8">
         <v>6232254</v>
       </c>
+      <c r="AE90" t="s">
+        <v>232</v>
+      </c>
     </row>
-    <row r="91" spans="1:30">
+    <row r="91" spans="1:31">
       <c r="A91" t="s">
         <v>96</v>
       </c>
@@ -9979,8 +10298,11 @@
       <c r="AD91" s="8">
         <v>6232254</v>
       </c>
+      <c r="AE91" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="92" spans="1:30">
+    <row r="92" spans="1:31">
       <c r="A92" t="s">
         <v>97</v>
       </c>
@@ -10071,8 +10393,11 @@
       <c r="AD92" s="7">
         <v>6222128</v>
       </c>
+      <c r="AE92" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="93" spans="1:30">
+    <row r="93" spans="1:31">
       <c r="A93" t="s">
         <v>99</v>
       </c>
@@ -10163,8 +10488,11 @@
       <c r="AD93" s="7">
         <v>6222128</v>
       </c>
+      <c r="AE93" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="94" spans="1:30">
+    <row r="94" spans="1:31">
       <c r="A94" t="s">
         <v>100</v>
       </c>
@@ -10255,8 +10583,11 @@
       <c r="AD94" s="7">
         <v>6221754</v>
       </c>
+      <c r="AE94" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="95" spans="1:30">
+    <row r="95" spans="1:31">
       <c r="A95" t="s">
         <v>101</v>
       </c>
@@ -10347,8 +10678,11 @@
       <c r="AD95" s="7">
         <v>6221349</v>
       </c>
+      <c r="AE95" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="96" spans="1:30">
+    <row r="96" spans="1:31">
       <c r="A96" t="s">
         <v>102</v>
       </c>
@@ -10439,8 +10773,11 @@
       <c r="AD96" s="7">
         <v>6220801</v>
       </c>
+      <c r="AE96" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="97" spans="1:30">
+    <row r="97" spans="1:31">
       <c r="A97" t="s">
         <v>103</v>
       </c>
@@ -10531,8 +10868,11 @@
       <c r="AD97" s="7">
         <v>6220801</v>
       </c>
+      <c r="AE97" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="98" spans="1:30">
+    <row r="98" spans="1:31">
       <c r="A98" t="s">
         <v>104</v>
       </c>
@@ -10623,8 +10963,11 @@
       <c r="AD98" s="7">
         <v>6220494</v>
       </c>
+      <c r="AE98" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="99" spans="1:30">
+    <row r="99" spans="1:31">
       <c r="A99" t="s">
         <v>105</v>
       </c>
@@ -10715,8 +11058,11 @@
       <c r="AD99" s="7">
         <v>6220494</v>
       </c>
+      <c r="AE99" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="100" spans="1:30">
+    <row r="100" spans="1:31">
       <c r="A100" t="s">
         <v>106</v>
       </c>
@@ -10807,8 +11153,11 @@
       <c r="AD100" s="7">
         <v>6220494</v>
       </c>
+      <c r="AE100" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="101" spans="1:30">
+    <row r="101" spans="1:31">
       <c r="A101" t="s">
         <v>107</v>
       </c>
@@ -10899,8 +11248,11 @@
       <c r="AD101" s="7">
         <v>6220494</v>
       </c>
+      <c r="AE101" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="102" spans="1:30">
+    <row r="102" spans="1:31">
       <c r="A102" t="s">
         <v>108</v>
       </c>
@@ -10991,8 +11343,11 @@
       <c r="AD102" s="7">
         <v>6220312</v>
       </c>
+      <c r="AE102" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="103" spans="1:30">
+    <row r="103" spans="1:31">
       <c r="A103" t="s">
         <v>109</v>
       </c>
@@ -11083,8 +11438,11 @@
       <c r="AD103" s="7">
         <v>6220312</v>
       </c>
+      <c r="AE103" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="104" spans="1:30">
+    <row r="104" spans="1:31">
       <c r="A104" t="s">
         <v>110</v>
       </c>
@@ -11175,8 +11533,11 @@
       <c r="AD104" s="7">
         <v>6220312</v>
       </c>
+      <c r="AE104" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="105" spans="1:30">
+    <row r="105" spans="1:31">
       <c r="A105" t="s">
         <v>111</v>
       </c>
@@ -11267,8 +11628,11 @@
       <c r="AD105" s="7">
         <v>6220312</v>
       </c>
+      <c r="AE105" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="106" spans="1:30">
+    <row r="106" spans="1:31">
       <c r="A106" t="s">
         <v>112</v>
       </c>
@@ -11359,8 +11723,11 @@
       <c r="AD106" s="7">
         <v>6220312</v>
       </c>
+      <c r="AE106" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="107" spans="1:30">
+    <row r="107" spans="1:31">
       <c r="A107" t="s">
         <v>113</v>
       </c>
@@ -11451,8 +11818,11 @@
       <c r="AD107" s="7">
         <v>6219982</v>
       </c>
+      <c r="AE107" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="108" spans="1:30">
+    <row r="108" spans="1:31">
       <c r="A108" t="s">
         <v>114</v>
       </c>
@@ -11543,8 +11913,11 @@
       <c r="AD108" s="7">
         <v>6219982</v>
       </c>
+      <c r="AE108" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="109" spans="1:30">
+    <row r="109" spans="1:31">
       <c r="A109" t="s">
         <v>115</v>
       </c>
@@ -11635,8 +12008,11 @@
       <c r="AD109" s="7">
         <v>6219665</v>
       </c>
+      <c r="AE109" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="110" spans="1:30">
+    <row r="110" spans="1:31">
       <c r="A110" t="s">
         <v>116</v>
       </c>
@@ -11727,8 +12103,11 @@
       <c r="AD110" s="7">
         <v>6219665</v>
       </c>
+      <c r="AE110" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="111" spans="1:30">
+    <row r="111" spans="1:31">
       <c r="A111" t="s">
         <v>117</v>
       </c>
@@ -11819,8 +12198,11 @@
       <c r="AD111" s="7">
         <v>6219665</v>
       </c>
+      <c r="AE111" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="112" spans="1:30">
+    <row r="112" spans="1:31">
       <c r="A112" t="s">
         <v>118</v>
       </c>
@@ -11911,8 +12293,11 @@
       <c r="AD112" s="7">
         <v>6219375</v>
       </c>
+      <c r="AE112" t="s">
+        <v>231</v>
+      </c>
     </row>
-    <row r="113" spans="1:30">
+    <row r="113" spans="1:31">
       <c r="A113" t="s">
         <v>119</v>
       </c>
@@ -12003,8 +12388,11 @@
       <c r="AD113" s="7">
         <v>6219375</v>
       </c>
+      <c r="AE113" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="114" spans="1:30">
+    <row r="114" spans="1:31">
       <c r="A114" t="s">
         <v>120</v>
       </c>
@@ -12095,8 +12483,11 @@
       <c r="AD114" s="7">
         <v>6219375</v>
       </c>
+      <c r="AE114" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="115" spans="1:30">
+    <row r="115" spans="1:31">
       <c r="A115" t="s">
         <v>121</v>
       </c>
@@ -12187,8 +12578,11 @@
       <c r="AD115" s="8">
         <v>6219322</v>
       </c>
+      <c r="AE115" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="116" spans="1:30">
+    <row r="116" spans="1:31">
       <c r="A116" t="s">
         <v>122</v>
       </c>
@@ -12279,8 +12673,11 @@
       <c r="AD116" s="8">
         <v>6219322</v>
       </c>
+      <c r="AE116" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="117" spans="1:30">
+    <row r="117" spans="1:31">
       <c r="A117" t="s">
         <v>123</v>
       </c>
@@ -12371,8 +12768,11 @@
       <c r="AD117" s="8">
         <v>6219322</v>
       </c>
+      <c r="AE117" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="118" spans="1:30">
+    <row r="118" spans="1:31">
       <c r="A118" t="s">
         <v>124</v>
       </c>
@@ -12463,8 +12863,11 @@
       <c r="AD118" s="8">
         <v>6219322</v>
       </c>
+      <c r="AE118" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="119" spans="1:30">
+    <row r="119" spans="1:31">
       <c r="A119" t="s">
         <v>125</v>
       </c>
@@ -12555,8 +12958,11 @@
       <c r="AD119" s="8">
         <v>6219322</v>
       </c>
+      <c r="AE119" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="120" spans="1:30">
+    <row r="120" spans="1:31">
       <c r="A120" t="s">
         <v>126</v>
       </c>
@@ -12647,8 +13053,11 @@
       <c r="AD120" s="8">
         <v>6219322</v>
       </c>
+      <c r="AE120" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="121" spans="1:30">
+    <row r="121" spans="1:31">
       <c r="A121" t="s">
         <v>127</v>
       </c>
@@ -12739,8 +13148,11 @@
       <c r="AD121" s="8">
         <v>6219322</v>
       </c>
+      <c r="AE121" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="122" spans="1:30">
+    <row r="122" spans="1:31">
       <c r="A122" t="s">
         <v>128</v>
       </c>
@@ -12831,8 +13243,11 @@
       <c r="AD122" s="7">
         <v>6234933</v>
       </c>
+      <c r="AE122" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="123" spans="1:30">
+    <row r="123" spans="1:31">
       <c r="A123" t="s">
         <v>131</v>
       </c>
@@ -12923,8 +13338,11 @@
       <c r="AD123" s="7">
         <v>6236343</v>
       </c>
+      <c r="AE123" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="124" spans="1:30">
+    <row r="124" spans="1:31">
       <c r="A124" t="s">
         <v>132</v>
       </c>
@@ -13015,8 +13433,11 @@
       <c r="AD124" s="7">
         <v>6236343</v>
       </c>
+      <c r="AE124" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="125" spans="1:30">
+    <row r="125" spans="1:31">
       <c r="A125" t="s">
         <v>133</v>
       </c>
@@ -13107,8 +13528,11 @@
       <c r="AD125" s="7">
         <v>6234933</v>
       </c>
+      <c r="AE125" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="126" spans="1:30">
+    <row r="126" spans="1:31">
       <c r="A126" t="s">
         <v>134</v>
       </c>
@@ -13199,8 +13623,11 @@
       <c r="AD126" s="7">
         <v>6236343</v>
       </c>
+      <c r="AE126" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="127" spans="1:30">
+    <row r="127" spans="1:31">
       <c r="A127" t="s">
         <v>135</v>
       </c>
@@ -13291,8 +13718,11 @@
       <c r="AD127" s="7">
         <v>6238820</v>
       </c>
+      <c r="AE127" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="128" spans="1:30">
+    <row r="128" spans="1:31">
       <c r="A128" t="s">
         <v>136</v>
       </c>
@@ -13383,8 +13813,11 @@
       <c r="AD128" s="7">
         <v>6238820</v>
       </c>
+      <c r="AE128" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="129" spans="1:30">
+    <row r="129" spans="1:31">
       <c r="A129" t="s">
         <v>137</v>
       </c>
@@ -13475,8 +13908,11 @@
       <c r="AD129" s="7">
         <v>6238820</v>
       </c>
+      <c r="AE129" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="130" spans="1:30">
+    <row r="130" spans="1:31">
       <c r="A130" t="s">
         <v>138</v>
       </c>
@@ -13567,8 +14003,11 @@
       <c r="AD130" s="7">
         <v>6238820</v>
       </c>
+      <c r="AE130" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="131" spans="1:30">
+    <row r="131" spans="1:31">
       <c r="A131" t="s">
         <v>139</v>
       </c>
@@ -13659,8 +14098,11 @@
       <c r="AD131" s="7">
         <v>6238820</v>
       </c>
+      <c r="AE131" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="132" spans="1:30">
+    <row r="132" spans="1:31">
       <c r="A132" t="s">
         <v>140</v>
       </c>
@@ -13751,8 +14193,11 @@
       <c r="AD132" s="7">
         <v>6238820</v>
       </c>
+      <c r="AE132" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="133" spans="1:30">
+    <row r="133" spans="1:31">
       <c r="A133" t="s">
         <v>141</v>
       </c>
@@ -13843,8 +14288,11 @@
       <c r="AD133" s="7">
         <v>6238820</v>
       </c>
+      <c r="AE133" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="134" spans="1:30">
+    <row r="134" spans="1:31">
       <c r="A134" t="s">
         <v>142</v>
       </c>
@@ -13935,8 +14383,11 @@
       <c r="AD134" s="7">
         <v>6238820</v>
       </c>
+      <c r="AE134" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="135" spans="1:30">
+    <row r="135" spans="1:31">
       <c r="A135" t="s">
         <v>143</v>
       </c>
@@ -14027,8 +14478,11 @@
       <c r="AD135" s="7">
         <v>6238820</v>
       </c>
+      <c r="AE135" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="136" spans="1:30">
+    <row r="136" spans="1:31">
       <c r="A136" t="s">
         <v>144</v>
       </c>
@@ -14119,8 +14573,11 @@
       <c r="AD136" s="7">
         <v>6238820</v>
       </c>
+      <c r="AE136" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="137" spans="1:30">
+    <row r="137" spans="1:31">
       <c r="A137" t="s">
         <v>145</v>
       </c>
@@ -14211,8 +14668,11 @@
       <c r="AD137" s="7">
         <v>6238820</v>
       </c>
+      <c r="AE137" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="138" spans="1:30">
+    <row r="138" spans="1:31">
       <c r="A138" t="s">
         <v>146</v>
       </c>
@@ -14303,8 +14763,11 @@
       <c r="AD138" s="7">
         <v>6238820</v>
       </c>
+      <c r="AE138" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="139" spans="1:30">
+    <row r="139" spans="1:31">
       <c r="A139" t="s">
         <v>147</v>
       </c>
@@ -14395,8 +14858,11 @@
       <c r="AD139" s="7">
         <v>6236329</v>
       </c>
+      <c r="AE139" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="140" spans="1:30">
+    <row r="140" spans="1:31">
       <c r="A140" t="s">
         <v>148</v>
       </c>
@@ -14487,8 +14953,11 @@
       <c r="AD140" s="7">
         <v>6234571</v>
       </c>
+      <c r="AE140" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="141" spans="1:30">
+    <row r="141" spans="1:31">
       <c r="A141" t="s">
         <v>149</v>
       </c>
@@ -14579,8 +15048,11 @@
       <c r="AD141" s="7">
         <v>6234571</v>
       </c>
+      <c r="AE141" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="142" spans="1:30">
+    <row r="142" spans="1:31">
       <c r="A142" t="s">
         <v>150</v>
       </c>
@@ -14671,8 +15143,11 @@
       <c r="AD142" s="7">
         <v>6233644</v>
       </c>
+      <c r="AE142" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="143" spans="1:30">
+    <row r="143" spans="1:31">
       <c r="A143" t="s">
         <v>151</v>
       </c>
@@ -14763,8 +15238,11 @@
       <c r="AD143" s="7">
         <v>6234571</v>
       </c>
+      <c r="AE143" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="144" spans="1:30">
+    <row r="144" spans="1:31">
       <c r="A144" t="s">
         <v>152</v>
       </c>
@@ -14855,8 +15333,11 @@
       <c r="AD144" s="7">
         <v>6233644</v>
       </c>
+      <c r="AE144" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="145" spans="1:30">
+    <row r="145" spans="1:31">
       <c r="A145" t="s">
         <v>153</v>
       </c>
@@ -14947,8 +15428,11 @@
       <c r="AD145" s="7">
         <v>6233644</v>
       </c>
+      <c r="AE145" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="146" spans="1:30">
+    <row r="146" spans="1:31">
       <c r="A146" t="s">
         <v>154</v>
       </c>
@@ -15039,8 +15523,11 @@
       <c r="AD146" s="7">
         <v>6231207</v>
       </c>
+      <c r="AE146" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="147" spans="1:30">
+    <row r="147" spans="1:31">
       <c r="A147" t="s">
         <v>155</v>
       </c>
@@ -15131,8 +15618,11 @@
       <c r="AD147" s="7">
         <v>6236329</v>
       </c>
+      <c r="AE147" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="148" spans="1:30">
+    <row r="148" spans="1:31">
       <c r="A148" t="s">
         <v>156</v>
       </c>
@@ -15223,8 +15713,11 @@
       <c r="AD148" s="7">
         <v>6236329</v>
       </c>
+      <c r="AE148" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="149" spans="1:30">
+    <row r="149" spans="1:31">
       <c r="A149" t="s">
         <v>157</v>
       </c>
@@ -15315,8 +15808,11 @@
       <c r="AD149" s="7">
         <v>6236329</v>
       </c>
+      <c r="AE149" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="150" spans="1:30">
+    <row r="150" spans="1:31">
       <c r="A150" t="s">
         <v>158</v>
       </c>
@@ -15407,8 +15903,11 @@
       <c r="AD150" s="7">
         <v>6236329</v>
       </c>
+      <c r="AE150" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="151" spans="1:30">
+    <row r="151" spans="1:31">
       <c r="A151" t="s">
         <v>159</v>
       </c>
@@ -15499,8 +15998,11 @@
       <c r="AD151" s="7">
         <v>6236329</v>
       </c>
+      <c r="AE151" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="152" spans="1:30">
+    <row r="152" spans="1:31">
       <c r="A152" t="s">
         <v>160</v>
       </c>
@@ -15591,8 +16093,11 @@
       <c r="AD152" s="7">
         <v>6231207</v>
       </c>
+      <c r="AE152" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="153" spans="1:30">
+    <row r="153" spans="1:31">
       <c r="A153" t="s">
         <v>161</v>
       </c>
@@ -15683,8 +16188,11 @@
       <c r="AD153" s="7">
         <v>6230131</v>
       </c>
+      <c r="AE153" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="154" spans="1:30">
+    <row r="154" spans="1:31">
       <c r="A154" t="s">
         <v>162</v>
       </c>
@@ -15775,8 +16283,11 @@
       <c r="AD154" s="7">
         <v>6230131</v>
       </c>
+      <c r="AE154" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="155" spans="1:30">
+    <row r="155" spans="1:31">
       <c r="A155" t="s">
         <v>163</v>
       </c>
@@ -15867,8 +16378,11 @@
       <c r="AD155" s="7">
         <v>6231207</v>
       </c>
+      <c r="AE155" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="156" spans="1:30">
+    <row r="156" spans="1:31">
       <c r="A156" t="s">
         <v>164</v>
       </c>
@@ -15959,8 +16473,11 @@
       <c r="AD156" s="7">
         <v>6230131</v>
       </c>
+      <c r="AE156" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="157" spans="1:30">
+    <row r="157" spans="1:31">
       <c r="A157" t="s">
         <v>165</v>
       </c>
@@ -16051,8 +16568,11 @@
       <c r="AD157" s="7">
         <v>6230131</v>
       </c>
+      <c r="AE157" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="158" spans="1:30">
+    <row r="158" spans="1:31">
       <c r="A158" t="s">
         <v>166</v>
       </c>
@@ -16143,8 +16663,11 @@
       <c r="AD158" s="7">
         <v>6231805</v>
       </c>
+      <c r="AE158" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="159" spans="1:30">
+    <row r="159" spans="1:31">
       <c r="A159" t="s">
         <v>167</v>
       </c>
@@ -16235,8 +16758,11 @@
       <c r="AD159" s="7">
         <v>6231805</v>
       </c>
+      <c r="AE159" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="160" spans="1:30">
+    <row r="160" spans="1:31">
       <c r="A160" t="s">
         <v>168</v>
       </c>
@@ -16327,8 +16853,11 @@
       <c r="AD160" s="7">
         <v>6231805</v>
       </c>
+      <c r="AE160" t="s">
+        <v>228</v>
+      </c>
     </row>
-    <row r="161" spans="1:30">
+    <row r="161" spans="1:31">
       <c r="A161" t="s">
         <v>169</v>
       </c>
@@ -16419,8 +16948,11 @@
       <c r="AD161" s="7">
         <v>6230569</v>
       </c>
+      <c r="AE161" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="162" spans="1:30">
+    <row r="162" spans="1:31">
       <c r="A162" t="s">
         <v>170</v>
       </c>
@@ -16511,8 +17043,11 @@
       <c r="AD162" s="8">
         <v>6230127</v>
       </c>
+      <c r="AE162" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="163" spans="1:30">
+    <row r="163" spans="1:31">
       <c r="A163" t="s">
         <v>172</v>
       </c>
@@ -16603,8 +17138,11 @@
       <c r="AD163" s="8">
         <v>6230127</v>
       </c>
+      <c r="AE163" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="164" spans="1:30">
+    <row r="164" spans="1:31">
       <c r="A164" t="s">
         <v>173</v>
       </c>
@@ -16695,8 +17233,11 @@
       <c r="AD164" s="8">
         <v>6230127</v>
       </c>
+      <c r="AE164" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="165" spans="1:30">
+    <row r="165" spans="1:31">
       <c r="A165" t="s">
         <v>174</v>
       </c>
@@ -16787,8 +17328,11 @@
       <c r="AD165" s="8">
         <v>6230127</v>
       </c>
+      <c r="AE165" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="166" spans="1:30">
+    <row r="166" spans="1:31">
       <c r="A166" t="s">
         <v>175</v>
       </c>
@@ -16879,8 +17423,11 @@
       <c r="AD166" s="8">
         <v>6230127</v>
       </c>
+      <c r="AE166" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="167" spans="1:30">
+    <row r="167" spans="1:31">
       <c r="A167" t="s">
         <v>176</v>
       </c>
@@ -16971,8 +17518,11 @@
       <c r="AD167" s="8">
         <v>6230127</v>
       </c>
+      <c r="AE167" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="168" spans="1:30">
+    <row r="168" spans="1:31">
       <c r="A168" t="s">
         <v>177</v>
       </c>
@@ -17063,8 +17613,11 @@
       <c r="AD168" s="8">
         <v>6230127</v>
       </c>
+      <c r="AE168" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="169" spans="1:30">
+    <row r="169" spans="1:31">
       <c r="A169" t="s">
         <v>178</v>
       </c>
@@ -17155,8 +17708,11 @@
       <c r="AD169" s="8">
         <v>6230127</v>
       </c>
+      <c r="AE169" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="170" spans="1:30">
+    <row r="170" spans="1:31">
       <c r="A170" t="s">
         <v>179</v>
       </c>
@@ -17247,8 +17803,11 @@
       <c r="AD170" s="8">
         <v>6230127</v>
       </c>
+      <c r="AE170" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="171" spans="1:30">
+    <row r="171" spans="1:31">
       <c r="A171" t="s">
         <v>180</v>
       </c>
@@ -17339,8 +17898,11 @@
       <c r="AD171" s="8">
         <v>6230127</v>
       </c>
+      <c r="AE171" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="172" spans="1:30">
+    <row r="172" spans="1:31">
       <c r="A172" t="s">
         <v>181</v>
       </c>
@@ -17431,8 +17993,11 @@
       <c r="AD172" s="8">
         <v>6230127</v>
       </c>
+      <c r="AE172" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="173" spans="1:30">
+    <row r="173" spans="1:31">
       <c r="A173" t="s">
         <v>182</v>
       </c>
@@ -17523,8 +18088,11 @@
       <c r="AD173" s="8">
         <v>6230127</v>
       </c>
+      <c r="AE173" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="174" spans="1:30">
+    <row r="174" spans="1:31">
       <c r="A174" t="s">
         <v>183</v>
       </c>
@@ -17615,8 +18183,11 @@
       <c r="AD174" s="8">
         <v>6230127</v>
       </c>
+      <c r="AE174" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="175" spans="1:30">
+    <row r="175" spans="1:31">
       <c r="A175" t="s">
         <v>184</v>
       </c>
@@ -17707,8 +18278,11 @@
       <c r="AD175" s="8">
         <v>6230127</v>
       </c>
+      <c r="AE175" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="176" spans="1:30">
+    <row r="176" spans="1:31">
       <c r="A176" t="s">
         <v>185</v>
       </c>
@@ -17799,8 +18373,11 @@
       <c r="AD176" s="8">
         <v>6236426</v>
       </c>
+      <c r="AE176" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="177" spans="1:30">
+    <row r="177" spans="1:31">
       <c r="A177" t="s">
         <v>186</v>
       </c>
@@ -17891,8 +18468,11 @@
       <c r="AD177" s="8">
         <v>6236426</v>
       </c>
+      <c r="AE177" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="178" spans="1:30">
+    <row r="178" spans="1:31">
       <c r="A178" t="s">
         <v>187</v>
       </c>
@@ -17983,8 +18563,11 @@
       <c r="AD178" s="8">
         <v>6233405</v>
       </c>
+      <c r="AE178" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="179" spans="1:30">
+    <row r="179" spans="1:31">
       <c r="A179" s="2" t="s">
         <v>188</v>
       </c>
@@ -18075,8 +18658,11 @@
       <c r="AD179" s="8">
         <v>6233405</v>
       </c>
+      <c r="AE179" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="180" spans="1:30">
+    <row r="180" spans="1:31">
       <c r="A180" t="s">
         <v>189</v>
       </c>
@@ -18167,8 +18753,11 @@
       <c r="AD180" s="8">
         <v>6233405</v>
       </c>
+      <c r="AE180" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="181" spans="1:30">
+    <row r="181" spans="1:31">
       <c r="A181" t="s">
         <v>190</v>
       </c>
@@ -18259,8 +18848,11 @@
       <c r="AD181" s="8">
         <v>6233405</v>
       </c>
+      <c r="AE181" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="182" spans="1:30">
+    <row r="182" spans="1:31">
       <c r="A182" t="s">
         <v>191</v>
       </c>
@@ -18351,8 +18943,11 @@
       <c r="AD182" s="8">
         <v>6233405</v>
       </c>
+      <c r="AE182" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="183" spans="1:30">
+    <row r="183" spans="1:31">
       <c r="A183" t="s">
         <v>192</v>
       </c>
@@ -18443,8 +19038,11 @@
       <c r="AD183" s="8">
         <v>6233405</v>
       </c>
+      <c r="AE183" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="184" spans="1:30">
+    <row r="184" spans="1:31">
       <c r="A184" t="s">
         <v>193</v>
       </c>
@@ -18535,8 +19133,11 @@
       <c r="AD184" s="8">
         <v>6233405</v>
       </c>
+      <c r="AE184" t="s">
+        <v>230</v>
+      </c>
     </row>
-    <row r="185" spans="1:30">
+    <row r="185" spans="1:31">
       <c r="A185" t="s">
         <v>194</v>
       </c>
@@ -18627,8 +19228,11 @@
       <c r="AD185" s="8">
         <v>6233405</v>
       </c>
+      <c r="AE185" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="186" spans="1:30">
+    <row r="186" spans="1:31">
       <c r="A186" t="s">
         <v>195</v>
       </c>
@@ -18719,8 +19323,11 @@
       <c r="AD186" s="8">
         <v>6233405</v>
       </c>
+      <c r="AE186" t="s">
+        <v>229</v>
+      </c>
     </row>
-    <row r="187" spans="1:30">
+    <row r="187" spans="1:31">
       <c r="A187" t="s">
         <v>196</v>
       </c>
@@ -18811,8 +19418,11 @@
       <c r="AD187" s="8">
         <v>6236426</v>
       </c>
+      <c r="AE187" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="188" spans="1:30">
+    <row r="188" spans="1:31">
       <c r="A188" t="s">
         <v>197</v>
       </c>
@@ -18903,8 +19513,11 @@
       <c r="AD188" s="8">
         <v>6236426</v>
       </c>
+      <c r="AE188" t="s">
+        <v>227</v>
+      </c>
     </row>
-    <row r="189" spans="1:30">
+    <row r="189" spans="1:31">
       <c r="A189" t="s">
         <v>198</v>
       </c>
@@ -18995,8 +19608,11 @@
       <c r="AD189" s="8">
         <v>6236426</v>
       </c>
+      <c r="AE189" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="190" spans="1:30">
+    <row r="190" spans="1:31">
       <c r="A190" t="s">
         <v>199</v>
       </c>
@@ -19087,8 +19703,11 @@
       <c r="AD190" s="8">
         <v>6236426</v>
       </c>
+      <c r="AE190" t="s">
+        <v>234</v>
+      </c>
     </row>
-    <row r="191" spans="1:30">
+    <row r="191" spans="1:31">
       <c r="A191" t="s">
         <v>200</v>
       </c>
@@ -19179,9 +19798,12 @@
       <c r="AD191" s="8">
         <v>6236426</v>
       </c>
+      <c r="AE191" t="s">
+        <v>229</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:AD191"/>
+  <autoFilter ref="A1:AE191"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>

</xml_diff>